<commit_message>
Invalidate formula caches after render.
So that formulas which reference templated cells will be recalculated the next time an application opens the workbook.
</commit_message>
<xml_diff>
--- a/spec/fixtures/xlsx/placeholders.xlsx
+++ b/spec/fixtures/xlsx/placeholders.xlsx
@@ -488,7 +488,7 @@
       <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14:K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.31"/>
   </cols>
@@ -671,7 +671,50 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K21" s="4"/>
+      <c r="A21" s="0" t="n">
+        <f aca="false">AVERAGE(A18:A20)</f>
+        <v>1</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <f aca="false">AVERAGE(B18:B20)</f>
+        <v>44132</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <f aca="false">AVERAGE(C18:C20)</f>
+        <v>7</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">AVERAGE(D18:D20)</f>
+        <v>3.141528</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <f aca="false">COUNT(E18:E20)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="0" t="e">
+        <f aca="false">AVERAGE(F18:F20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G21" s="0" t="e">
+        <f aca="false">AVERAGE(G18:G20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H21" s="0" t="e">
+        <f aca="false">AVERAGE(H18:H20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I21" s="0" t="e">
+        <f aca="false">AVERAGE(I18:I20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J21" s="0" t="e">
+        <f aca="false">AVERAGE(J18:J20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K21" s="0" t="e">
+        <f aca="false">AVERAGE(K18:K20)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">

</xml_diff>

<commit_message>
generalise sorting of sheet child tags, and use for sorting rows and cells
</commit_message>
<xml_diff>
--- a/spec/fixtures/xlsx/placeholders.xlsx
+++ b/spec/fixtures/xlsx/placeholders.xlsx
@@ -182,13 +182,13 @@
     <t xml:space="preserve">Controller</t>
   </si>
   <si>
+    <t xml:space="preserve">{{logo|133x100}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{logo}}</t>
+  </si>
+  <si>
     <t xml:space="preserve">{{streams|tabular}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{logo|133x100}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{logo}}</t>
   </si>
   <si>
     <t xml:space="preserve">Manual Table</t>
@@ -431,6 +431,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -440,10 +444,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -485,10 +485,10 @@
   <dimension ref="A5:K26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14:K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.31"/>
   </cols>
@@ -624,6 +624,12 @@
       <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="H14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
@@ -635,26 +641,26 @@
       <c r="A17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
+      <c r="A18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="n">
+      <c r="A19" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="B19" s="6" t="n">
+      <c r="B19" s="7" t="n">
         <v>44132</v>
       </c>
       <c r="C19" s="0" t="n">
@@ -664,22 +670,14 @@
         <v>3.141528</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H20" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K21" s="7"/>
+      <c r="K21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="K22" s="7"/>
+      <c r="K22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
@@ -744,10 +742,10 @@
       <c r="I24" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="J24" s="7" t="s">
+      <c r="J24" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K24" s="7" t="s">
+      <c r="K24" s="4" t="s">
         <v>57</v>
       </c>
     </row>
@@ -835,7 +833,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
remove table parts causing excel to have indigestion from test output
</commit_message>
<xml_diff>
--- a/spec/fixtures/xlsx/placeholders.xlsx
+++ b/spec/fixtures/xlsx/placeholders.xlsx
@@ -459,24 +459,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="chart_data" displayName="chart_data" ref="A19:K24" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <tableColumns count="11">
-    <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2"/>
-    <tableColumn id="3" name="Column3"/>
-    <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Column5"/>
-    <tableColumn id="6" name="Column6"/>
-    <tableColumn id="7" name="Column7"/>
-    <tableColumn id="8" name="Column8"/>
-    <tableColumn id="9" name="Column9"/>
-    <tableColumn id="10" name="Column10"/>
-    <tableColumn id="11" name="Column11"/>
-  </tableColumns>
-</table>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -881,8 +863,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <tableParts>
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>